<commit_message>
Refactor custom property resolver test
</commit_message>
<xml_diff>
--- a/src/Robintty.Npoi.Mapper.Tests/Book1.xlsx
+++ b/src/Robintty.Npoi.Mapper.Tests/Book1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\src\github\Npoi.Mapper\Npoi.Mapper\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\source\repos\Npoi.Mapper\src\Robintty.Npoi.Mapper.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA126030-F499-489A-B1DF-4F0A0822DE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="0" windowWidth="24120" windowHeight="12795" activeTab="6"/>
+    <workbookView xWindow="8120" yWindow="2570" windowWidth="28830" windowHeight="15400" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESources" sheetId="2" r:id="rId1"/>
@@ -19,6 +20,7 @@
     <sheet name="Backlogs" sheetId="4" r:id="rId5"/>
     <sheet name="TestClass" sheetId="6" r:id="rId6"/>
     <sheet name="NullableClass" sheetId="7" r:id="rId7"/>
+    <sheet name="RowHeader" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="77">
   <si>
     <t>Frank Wu</t>
   </si>
@@ -266,20 +268,50 @@
   <si>
     <t>d</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Creation Date</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Robert42</t>
+  </si>
+  <si>
+    <t>robert@gmail.com</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Adam28</t>
+  </si>
+  <si>
+    <t>adam@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\-yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -299,7 +331,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -307,7 +339,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -359,7 +391,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -367,7 +399,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -385,13 +417,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -702,21 +735,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49.375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="17.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.36328125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -724,7 +757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -732,7 +765,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,28 +776,28 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.25" customWidth="1"/>
+    <col min="1" max="1" width="32.26953125" customWidth="1"/>
     <col min="2" max="3" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -778,7 +811,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -792,7 +825,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -806,7 +839,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -820,7 +853,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -834,7 +867,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -848,7 +881,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -862,7 +895,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -876,7 +909,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -890,7 +923,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -904,7 +937,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -918,7 +951,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -939,22 +972,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="33.125" customWidth="1"/>
-    <col min="3" max="3" width="26.25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="36.375" customWidth="1"/>
+    <col min="2" max="2" width="33.08984375" customWidth="1"/>
+    <col min="3" max="3" width="26.26953125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="36.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -968,7 +1001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -982,7 +1015,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -996,7 +1029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1018,19 +1051,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="24.75" customWidth="1"/>
-    <col min="3" max="7" width="11.375" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+    <col min="3" max="7" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1053,7 +1086,7 @@
         <v>42583</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1076,7 +1109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -1096,7 +1129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +1152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -1147,24 +1180,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="4.25" customWidth="1"/>
-    <col min="2" max="2" width="47.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.25" customWidth="1"/>
-    <col min="5" max="5" width="19.875" customWidth="1"/>
-    <col min="6" max="6" width="50.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="2" max="2" width="47.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.90625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="19.90625" customWidth="1"/>
+    <col min="6" max="6" width="50.36328125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="7" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -1184,7 +1217,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="29">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1204,7 +1237,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -1212,7 +1245,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
@@ -1220,7 +1253,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -1228,7 +1261,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
@@ -1236,7 +1269,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
@@ -1244,7 +1277,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
@@ -1252,7 +1285,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
@@ -1260,7 +1293,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
@@ -1268,7 +1301,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
@@ -1276,7 +1309,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
@@ -1284,7 +1317,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -1292,7 +1325,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
@@ -1300,7 +1333,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
@@ -1308,7 +1341,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
@@ -1316,7 +1349,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
@@ -1324,7 +1357,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
@@ -1332,7 +1365,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
@@ -1340,7 +1373,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
@@ -1348,7 +1381,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -1356,7 +1389,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
@@ -1364,7 +1397,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
@@ -1372,7 +1405,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
@@ -1380,7 +1413,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
@@ -1388,7 +1421,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
@@ -1396,7 +1429,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
@@ -1404,7 +1437,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
@@ -1412,7 +1445,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
@@ -1427,20 +1460,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.5" customWidth="1"/>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1451,7 +1484,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1462,7 +1495,7 @@
         <v>0.56779999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1473,7 +1506,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1492,20 +1525,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1513,7 +1546,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="11">
         <v>42736</v>
       </c>
@@ -1521,7 +1554,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="12" t="s">
         <v>52</v>
       </c>
@@ -1529,7 +1562,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="12" t="s">
         <v>61</v>
       </c>
@@ -1537,7 +1570,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1550,4 +1583,83 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BA3DF3-DB46-4C90-8552-E5413A1A393B}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="11">
+        <v>27954</v>
+      </c>
+      <c r="C5" s="11">
+        <v>32153</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{5EFB49B9-4D1D-47F6-9E82-1B62F1634854}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{666C96D6-90E6-4D52-AE55-CF2329CBC633}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>